<commit_message>
Edit các quy định
</commit_message>
<xml_diff>
--- a/Reports/ref-Các quy định.xlsx
+++ b/Reports/ref-Các quy định.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coxan_000\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\Đồ án kì 1-2015\OOAD-2015\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -96,9 +96,6 @@
     <t>2. Điều kiện đổi trả:</t>
   </si>
   <si>
-    <t>1. Còn đầy đủ hóa đơn mua hàng (áp dụng với các đơn hàng mua trước ngày 1/6/2015)</t>
-  </si>
-  <si>
     <t>2. Còn đầy đủ hộp sản phẩm</t>
   </si>
   <si>
@@ -160,6 +157,9 @@
   </si>
   <si>
     <t>quý khách hàng có thể mang sản phẩm ra siêu thị để nhập trả và lấy lại 100% số tiền ( sản phẩm không nhất thiết phải còn bao bì).</t>
+  </si>
+  <si>
+    <t>1. Còn đầy đủ hóa đơn mua hàng (nếu có)</t>
   </si>
 </sst>
 </file>
@@ -400,33 +400,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -448,6 +421,33 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -732,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,19 +745,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="15"/>
+      <c r="A2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="6"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="14" t="s">
         <v>17</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -768,7 +768,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E4" s="6"/>
+      <c r="E4" s="15"/>
       <c r="F4" s="3" t="s">
         <v>3</v>
       </c>
@@ -777,7 +777,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E5" s="6"/>
+      <c r="E5" s="15"/>
       <c r="F5" s="3" t="s">
         <v>5</v>
       </c>
@@ -786,7 +786,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E6" s="6"/>
+      <c r="E6" s="15"/>
       <c r="F6" s="3" t="s">
         <v>7</v>
       </c>
@@ -795,7 +795,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E7" s="7"/>
+      <c r="E7" s="16"/>
       <c r="F7" s="3" t="s">
         <v>9</v>
       </c>
@@ -804,7 +804,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="14" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="4" t="s">
@@ -815,7 +815,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E9" s="6"/>
+      <c r="E9" s="15"/>
       <c r="F9" s="3" t="s">
         <v>3</v>
       </c>
@@ -824,7 +824,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E10" s="6"/>
+      <c r="E10" s="15"/>
       <c r="F10" s="3" t="s">
         <v>5</v>
       </c>
@@ -833,7 +833,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E11" s="6"/>
+      <c r="E11" s="15"/>
       <c r="F11" s="3" t="s">
         <v>7</v>
       </c>
@@ -842,7 +842,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E12" s="7"/>
+      <c r="E12" s="16"/>
       <c r="F12" s="3" t="s">
         <v>9</v>
       </c>
@@ -851,25 +851,25 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="11"/>
+      <c r="G13" s="20"/>
     </row>
     <row r="14" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E14" s="6"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="13"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="22"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E15" s="7"/>
-      <c r="F15" s="8" t="s">
+      <c r="E15" s="16"/>
+      <c r="F15" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="G15" s="9"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
@@ -877,96 +877,96 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
+      <c r="A18" s="5"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" s="16"/>
+      <c r="A27" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="7"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E30" s="8"/>
+      <c r="F30" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E30" s="17"/>
-      <c r="F30" s="18" t="s">
+    <row r="31" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="E31" s="9" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="E31" s="18" t="s">
+      <c r="F31" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F31" s="19" t="s">
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E32" s="9" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E32" s="18" t="s">
+      <c r="F32" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F32" s="19" t="s">
+    </row>
+    <row r="33" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E33" s="11" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E33" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F33" s="21" t="s">
-        <v>32</v>
+      <c r="F33" s="12" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E34" s="20"/>
-      <c r="F34" s="22"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="13"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -974,13 +974,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="E3:E7"/>
+    <mergeCell ref="F13:G14"/>
     <mergeCell ref="E33:E34"/>
     <mergeCell ref="F33:F34"/>
     <mergeCell ref="E8:E12"/>
     <mergeCell ref="E13:E15"/>
     <mergeCell ref="F15:G15"/>
-    <mergeCell ref="E3:E7"/>
-    <mergeCell ref="F13:G14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>